<commit_message>
:beers: Close #163 CM
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0/Analizzato TP NR CAMPAGNE COMMERCIALI.xlsx
+++ b/docs/tp/Sfera_4.0/Analizzato TP NR CAMPAGNE COMMERCIALI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Sfera_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB20D24-8276-481B-A597-9544FDEAA837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E322C71-01B6-4FA9-BB24-F600BCFF63F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{F4CA1F3C-0BA7-435E-BB88-9578C1AAF535}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:I7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -783,35 +783,44 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">

</xml_diff>